<commit_message>
Further works, before cleanup.
</commit_message>
<xml_diff>
--- a/keys_df.xlsx
+++ b/keys_df.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\MPIEA\projects\Dislikes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2694ABE-3330-4A9E-8677-205E48D32276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE475FC-36C0-48E4-8FDD-B66BAD105CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="key" sheetId="2" r:id="rId2"/>
-    <sheet name="keys2" sheetId="3" r:id="rId3"/>
+    <sheet name="fa_keys" sheetId="1" r:id="rId1"/>
+    <sheet name="keys_v1" sheetId="2" r:id="rId2"/>
+    <sheet name="keys_v2" sheetId="3" r:id="rId3"/>
+    <sheet name="keys_v3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="65">
   <si>
     <t>rowname</t>
   </si>
@@ -214,6 +215,9 @@
   </si>
   <si>
     <t>MR_too_balladesk</t>
+  </si>
+  <si>
+    <t>MR_too_complex</t>
   </si>
 </sst>
 </file>
@@ -1839,7 +1843,7 @@
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="A1:M42"/>
+      <selection activeCell="B1" sqref="B1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3580,8 +3584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5BC072-233F-4756-9898-2594F4655466}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E39" sqref="A1:K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5059,4 +5063,1363 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7ABA44F-6317-4B3E-84CA-096C2F839C7B}">
+  <dimension ref="A1:J42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H15" sqref="H1:H1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>